<commit_message>
added code to count plain and encrypted blocks per file
</commit_message>
<xml_diff>
--- a/analysis/naive/safe_write_predictions_naive.xlsx
+++ b/analysis/naive/safe_write_predictions_naive.xlsx
@@ -5,20 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fac_rubin/Documents/GeorgiaTech/CS_6727-Practicum/filesystem/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fac_rubin/Documents/GeorgiaTech/CS_6727-Practicum/filesystem/analysis/naive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F3584D-0A21-E942-9E01-07AA8BE065E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2C90BB-FD88-4E48-9A01-4DD802E7BD1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="2140" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{C6D897B8-16C8-7A4E-92A5-749E23A3A761}"/>
+    <workbookView xWindow="9200" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{C6D897B8-16C8-7A4E-92A5-749E23A3A761}"/>
   </bookViews>
   <sheets>
-    <sheet name="detected" sheetId="1" r:id="rId1"/>
-    <sheet name="runtime" sheetId="3" r:id="rId2"/>
-    <sheet name="raw" sheetId="2" r:id="rId3"/>
+    <sheet name="runtime" sheetId="3" r:id="rId1"/>
+    <sheet name="plaintext-detected" sheetId="1" r:id="rId2"/>
+    <sheet name="encrypted-detected" sheetId="5" r:id="rId3"/>
+    <sheet name="plaintext-raw" sheetId="2" r:id="rId4"/>
+    <sheet name="encrypted-raw" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="tmp" localSheetId="1">runtime!$A$1:$B$1459</definedName>
+    <definedName name="tmp" localSheetId="0">runtime!$A$1:$B$1459</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +34,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{DBA8C51C-FE89-994A-8518-C68BD7531D61}" name="tmp" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/fac_rubin/Documents/GeorgiaTech/CS_6727-Practicum/filesystem/tmp.csv" tab="0" delimiter=":">
+    <textPr sourceFile="/Users/fac_rubin/Documents/GeorgiaTech/CS_6727-Practicum/filesystem/tmp.csv" tab="0" delimiter=":">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1918" uniqueCount="247">
   <si>
     <t>encrypted</t>
   </si>
@@ -184,6 +186,606 @@
   </si>
   <si>
     <t>50,000X penalty!!</t>
+  </si>
+  <si>
+    <t>writing aes.test.apk</t>
+  </si>
+  <si>
+    <t>writing aes.test.app</t>
+  </si>
+  <si>
+    <t>writing aes.test.docx</t>
+  </si>
+  <si>
+    <t>writing aes.test.elf</t>
+  </si>
+  <si>
+    <t>writing aes.test.exe</t>
+  </si>
+  <si>
+    <t>writing aes.test.gif</t>
+  </si>
+  <si>
+    <t>writing aes.test.html</t>
+  </si>
+  <si>
+    <t>writing aes.test.jpg</t>
+  </si>
+  <si>
+    <t>writing aes.test.mov</t>
+  </si>
+  <si>
+    <t>writing aes.test.mp3</t>
+  </si>
+  <si>
+    <t>writing aes.test.mp4</t>
+  </si>
+  <si>
+    <t>writing aes.test.o</t>
+  </si>
+  <si>
+    <t>writing aes.test.pdf</t>
+  </si>
+  <si>
+    <t>writing aes.test.png</t>
+  </si>
+  <si>
+    <t>writing aes.test.pptx</t>
+  </si>
+  <si>
+    <t>writing aes.test.tgz</t>
+  </si>
+  <si>
+    <t>writing aes.test.txt</t>
+  </si>
+  <si>
+    <t>writing aes.test.wav</t>
+  </si>
+  <si>
+    <t>writing aes.test.xlsx</t>
+  </si>
+  <si>
+    <t>writing aes.test.zip</t>
+  </si>
+  <si>
+    <t>writing bf.test.apk</t>
+  </si>
+  <si>
+    <t>writing bf.test.app</t>
+  </si>
+  <si>
+    <t>writing bf.test.docx</t>
+  </si>
+  <si>
+    <t>writing bf.test.elf</t>
+  </si>
+  <si>
+    <t>writing bf.test.exe</t>
+  </si>
+  <si>
+    <t>writing bf.test.gif</t>
+  </si>
+  <si>
+    <t>writing bf.test.html</t>
+  </si>
+  <si>
+    <t>writing bf.test.jpg</t>
+  </si>
+  <si>
+    <t>writing bf.test.mov</t>
+  </si>
+  <si>
+    <t>writing bf.test.mp3</t>
+  </si>
+  <si>
+    <t>writing bf.test.mp4</t>
+  </si>
+  <si>
+    <t>writing bf.test.o</t>
+  </si>
+  <si>
+    <t>writing bf.test.pdf</t>
+  </si>
+  <si>
+    <t>writing bf.test.png</t>
+  </si>
+  <si>
+    <t>writing bf.test.pptx</t>
+  </si>
+  <si>
+    <t>writing bf.test.tgz</t>
+  </si>
+  <si>
+    <t>writing bf.test.txt</t>
+  </si>
+  <si>
+    <t>writing bf.test.wav</t>
+  </si>
+  <si>
+    <t>writing bf.test.xlsx</t>
+  </si>
+  <si>
+    <t>writing bf.test.zip</t>
+  </si>
+  <si>
+    <t>writing cha.test.apk</t>
+  </si>
+  <si>
+    <t>writing cha.test.app</t>
+  </si>
+  <si>
+    <t>writing cha.test.docx</t>
+  </si>
+  <si>
+    <t>writing cha.test.elf</t>
+  </si>
+  <si>
+    <t>writing cha.test.exe</t>
+  </si>
+  <si>
+    <t>writing cha.test.gif</t>
+  </si>
+  <si>
+    <t>writing cha.test.html</t>
+  </si>
+  <si>
+    <t>writing cha.test.jpg</t>
+  </si>
+  <si>
+    <t>writing cha.test.mov</t>
+  </si>
+  <si>
+    <t>writing cha.test.mp3</t>
+  </si>
+  <si>
+    <t>writing cha.test.mp4</t>
+  </si>
+  <si>
+    <t>writing cha.test.o</t>
+  </si>
+  <si>
+    <t>writing cha.test.pdf</t>
+  </si>
+  <si>
+    <t>writing cha.test.png</t>
+  </si>
+  <si>
+    <t>writing cha.test.pptx</t>
+  </si>
+  <si>
+    <t>writing cha.test.tgz</t>
+  </si>
+  <si>
+    <t>writing cha.test.txt</t>
+  </si>
+  <si>
+    <t>writing cha.test.wav</t>
+  </si>
+  <si>
+    <t>writing cha.test.xlsx</t>
+  </si>
+  <si>
+    <t>writing cha.test.zip</t>
+  </si>
+  <si>
+    <t>writing des3.test.apk</t>
+  </si>
+  <si>
+    <t>writing des3.test.app</t>
+  </si>
+  <si>
+    <t>writing des3.test.docx</t>
+  </si>
+  <si>
+    <t>writing des3.test.elf</t>
+  </si>
+  <si>
+    <t>writing des3.test.exe</t>
+  </si>
+  <si>
+    <t>writing des3.test.gif</t>
+  </si>
+  <si>
+    <t>writing des3.test.html</t>
+  </si>
+  <si>
+    <t>writing des3.test.jpg</t>
+  </si>
+  <si>
+    <t>writing des3.test.mov</t>
+  </si>
+  <si>
+    <t>writing des3.test.mp3</t>
+  </si>
+  <si>
+    <t>writing des3.test.mp4</t>
+  </si>
+  <si>
+    <t>writing des3.test.o</t>
+  </si>
+  <si>
+    <t>writing des3.test.pdf</t>
+  </si>
+  <si>
+    <t>writing des3.test.png</t>
+  </si>
+  <si>
+    <t>writing des3.test.pptx</t>
+  </si>
+  <si>
+    <t>writing des3.test.tgz</t>
+  </si>
+  <si>
+    <t>writing des3.test.txt</t>
+  </si>
+  <si>
+    <t>writing des3.test.wav</t>
+  </si>
+  <si>
+    <t>writing des3.test.xlsx</t>
+  </si>
+  <si>
+    <t>writing des3.test.zip</t>
+  </si>
+  <si>
+    <t>writing rc4.test.apk</t>
+  </si>
+  <si>
+    <t>writing rc4.test.app</t>
+  </si>
+  <si>
+    <t>writing rc4.test.docx</t>
+  </si>
+  <si>
+    <t>writing rc4.test.elf</t>
+  </si>
+  <si>
+    <t>writing rc4.test.exe</t>
+  </si>
+  <si>
+    <t>writing rc4.test.gif</t>
+  </si>
+  <si>
+    <t>writing rc4.test.html</t>
+  </si>
+  <si>
+    <t>writing rc4.test.jpg</t>
+  </si>
+  <si>
+    <t>writing rc4.test.mov</t>
+  </si>
+  <si>
+    <t>writing rc4.test.mp3</t>
+  </si>
+  <si>
+    <t>writing rc4.test.mp4</t>
+  </si>
+  <si>
+    <t>writing rc4.test.o</t>
+  </si>
+  <si>
+    <t>writing rc4.test.pdf</t>
+  </si>
+  <si>
+    <t>writing rc4.test.png</t>
+  </si>
+  <si>
+    <t>writing rc4.test.pptx</t>
+  </si>
+  <si>
+    <t>writing rc4.test.tgz</t>
+  </si>
+  <si>
+    <t>writing rc4.test.txt</t>
+  </si>
+  <si>
+    <t>writing rc4.test.wav</t>
+  </si>
+  <si>
+    <t>writing rc4.test.xlsx</t>
+  </si>
+  <si>
+    <t>writing rc4.test.zip</t>
+  </si>
+  <si>
+    <t>aes.test.apk</t>
+  </si>
+  <si>
+    <t>aes.test.app</t>
+  </si>
+  <si>
+    <t>aes.test.docx</t>
+  </si>
+  <si>
+    <t>aes.test.elf</t>
+  </si>
+  <si>
+    <t>aes.test.exe</t>
+  </si>
+  <si>
+    <t>aes.test.gif</t>
+  </si>
+  <si>
+    <t>aes.test.html</t>
+  </si>
+  <si>
+    <t>aes.test.jpg</t>
+  </si>
+  <si>
+    <t>aes.test.mov</t>
+  </si>
+  <si>
+    <t>aes.test.mp3</t>
+  </si>
+  <si>
+    <t>aes.test.mp4</t>
+  </si>
+  <si>
+    <t>aes.test.o</t>
+  </si>
+  <si>
+    <t>aes.test.pdf</t>
+  </si>
+  <si>
+    <t>aes.test.png</t>
+  </si>
+  <si>
+    <t>aes.test.pptx</t>
+  </si>
+  <si>
+    <t>aes.test.tgz</t>
+  </si>
+  <si>
+    <t>aes.test.txt</t>
+  </si>
+  <si>
+    <t>aes.test.wav</t>
+  </si>
+  <si>
+    <t>aes.test.xlsx</t>
+  </si>
+  <si>
+    <t>aes.test.zip</t>
+  </si>
+  <si>
+    <t>bf.test.apk</t>
+  </si>
+  <si>
+    <t>bf.test.app</t>
+  </si>
+  <si>
+    <t>bf.test.docx</t>
+  </si>
+  <si>
+    <t>bf.test.elf</t>
+  </si>
+  <si>
+    <t>bf.test.exe</t>
+  </si>
+  <si>
+    <t>bf.test.gif</t>
+  </si>
+  <si>
+    <t>bf.test.html</t>
+  </si>
+  <si>
+    <t>bf.test.jpg</t>
+  </si>
+  <si>
+    <t>bf.test.mov</t>
+  </si>
+  <si>
+    <t>bf.test.mp3</t>
+  </si>
+  <si>
+    <t>bf.test.mp4</t>
+  </si>
+  <si>
+    <t>bf.test.o</t>
+  </si>
+  <si>
+    <t>bf.test.pdf</t>
+  </si>
+  <si>
+    <t>bf.test.png</t>
+  </si>
+  <si>
+    <t>bf.test.pptx</t>
+  </si>
+  <si>
+    <t>bf.test.tgz</t>
+  </si>
+  <si>
+    <t>bf.test.txt</t>
+  </si>
+  <si>
+    <t>bf.test.wav</t>
+  </si>
+  <si>
+    <t>bf.test.xlsx</t>
+  </si>
+  <si>
+    <t>bf.test.zip</t>
+  </si>
+  <si>
+    <t>cha.test.apk</t>
+  </si>
+  <si>
+    <t>cha.test.app</t>
+  </si>
+  <si>
+    <t>cha.test.docx</t>
+  </si>
+  <si>
+    <t>cha.test.elf</t>
+  </si>
+  <si>
+    <t>cha.test.exe</t>
+  </si>
+  <si>
+    <t>cha.test.gif</t>
+  </si>
+  <si>
+    <t>cha.test.html</t>
+  </si>
+  <si>
+    <t>cha.test.jpg</t>
+  </si>
+  <si>
+    <t>cha.test.mov</t>
+  </si>
+  <si>
+    <t>cha.test.mp3</t>
+  </si>
+  <si>
+    <t>cha.test.mp4</t>
+  </si>
+  <si>
+    <t>cha.test.o</t>
+  </si>
+  <si>
+    <t>cha.test.pdf</t>
+  </si>
+  <si>
+    <t>cha.test.png</t>
+  </si>
+  <si>
+    <t>cha.test.pptx</t>
+  </si>
+  <si>
+    <t>cha.test.tgz</t>
+  </si>
+  <si>
+    <t>cha.test.txt</t>
+  </si>
+  <si>
+    <t>cha.test.wav</t>
+  </si>
+  <si>
+    <t>cha.test.xlsx</t>
+  </si>
+  <si>
+    <t>cha.test.zip</t>
+  </si>
+  <si>
+    <t>des3.test.apk</t>
+  </si>
+  <si>
+    <t>des3.test.app</t>
+  </si>
+  <si>
+    <t>des3.test.docx</t>
+  </si>
+  <si>
+    <t>des3.test.elf</t>
+  </si>
+  <si>
+    <t>des3.test.exe</t>
+  </si>
+  <si>
+    <t>des3.test.gif</t>
+  </si>
+  <si>
+    <t>des3.test.html</t>
+  </si>
+  <si>
+    <t>des3.test.jpg</t>
+  </si>
+  <si>
+    <t>des3.test.mov</t>
+  </si>
+  <si>
+    <t>des3.test.mp3</t>
+  </si>
+  <si>
+    <t>des3.test.mp4</t>
+  </si>
+  <si>
+    <t>des3.test.o</t>
+  </si>
+  <si>
+    <t>des3.test.pdf</t>
+  </si>
+  <si>
+    <t>des3.test.png</t>
+  </si>
+  <si>
+    <t>des3.test.pptx</t>
+  </si>
+  <si>
+    <t>des3.test.tgz</t>
+  </si>
+  <si>
+    <t>des3.test.txt</t>
+  </si>
+  <si>
+    <t>des3.test.wav</t>
+  </si>
+  <si>
+    <t>des3.test.xlsx</t>
+  </si>
+  <si>
+    <t>des3.test.zip</t>
+  </si>
+  <si>
+    <t>rc4.test.apk</t>
+  </si>
+  <si>
+    <t>rc4.test.app</t>
+  </si>
+  <si>
+    <t>rc4.test.docx</t>
+  </si>
+  <si>
+    <t>rc4.test.elf</t>
+  </si>
+  <si>
+    <t>rc4.test.exe</t>
+  </si>
+  <si>
+    <t>rc4.test.gif</t>
+  </si>
+  <si>
+    <t>rc4.test.html</t>
+  </si>
+  <si>
+    <t>rc4.test.jpg</t>
+  </si>
+  <si>
+    <t>rc4.test.mov</t>
+  </si>
+  <si>
+    <t>rc4.test.mp3</t>
+  </si>
+  <si>
+    <t>rc4.test.mp4</t>
+  </si>
+  <si>
+    <t>rc4.test.o</t>
+  </si>
+  <si>
+    <t>rc4.test.pdf</t>
+  </si>
+  <si>
+    <t>rc4.test.png</t>
+  </si>
+  <si>
+    <t>rc4.test.pptx</t>
+  </si>
+  <si>
+    <t>rc4.test.tgz</t>
+  </si>
+  <si>
+    <t>rc4.test.txt</t>
+  </si>
+  <si>
+    <t>rc4.test.wav</t>
+  </si>
+  <si>
+    <t>rc4.test.xlsx</t>
+  </si>
+  <si>
+    <t>rc4.test.zip</t>
   </si>
 </sst>
 </file>
@@ -547,156 +1149,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1302855-714D-1048-9062-B5A4A4F813DB}">
-  <dimension ref="A1:B22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B22">
-        <f>COUNTIF(B2:B21,"X") / 20</f>
-        <v>0.35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AD2641-593D-524F-A62F-7E528F7475AA}">
   <dimension ref="A1:F1459"/>
   <sheetViews>
@@ -12405,7 +12857,979 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1302855-714D-1048-9062-B5A4A4F813DB}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <f>COUNTIF(B2:B21,"X") / 20</f>
+        <v>0.35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F99DEA17-B755-6A48-9E25-6935167A2FDB}">
+  <dimension ref="A1:C100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1">
+        <f>COUNTIF(B:B,"X") / 100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>170</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>171</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>172</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>173</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>175</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>176</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>178</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>179</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>180</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>181</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>182</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>183</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>184</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>185</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>186</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>187</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>188</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>189</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>190</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>191</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>192</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>193</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>194</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>195</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>196</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>197</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>198</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>199</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>200</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>201</v>
+      </c>
+      <c r="B55" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>202</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>203</v>
+      </c>
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>204</v>
+      </c>
+      <c r="B58" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>205</v>
+      </c>
+      <c r="B59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>206</v>
+      </c>
+      <c r="B60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>207</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>208</v>
+      </c>
+      <c r="B62" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>209</v>
+      </c>
+      <c r="B63" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>210</v>
+      </c>
+      <c r="B64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>211</v>
+      </c>
+      <c r="B65" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>212</v>
+      </c>
+      <c r="B66" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>213</v>
+      </c>
+      <c r="B67" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>214</v>
+      </c>
+      <c r="B68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>215</v>
+      </c>
+      <c r="B69" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>216</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>217</v>
+      </c>
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>218</v>
+      </c>
+      <c r="B72" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>219</v>
+      </c>
+      <c r="B73" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>220</v>
+      </c>
+      <c r="B74" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>221</v>
+      </c>
+      <c r="B75" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>222</v>
+      </c>
+      <c r="B76" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>223</v>
+      </c>
+      <c r="B77" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>224</v>
+      </c>
+      <c r="B78" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>225</v>
+      </c>
+      <c r="B79" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>226</v>
+      </c>
+      <c r="B80" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>227</v>
+      </c>
+      <c r="B81" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>228</v>
+      </c>
+      <c r="B82" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>229</v>
+      </c>
+      <c r="B83" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>230</v>
+      </c>
+      <c r="B84" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>231</v>
+      </c>
+      <c r="B85" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>232</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>233</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>234</v>
+      </c>
+      <c r="B88" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>235</v>
+      </c>
+      <c r="B89" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>236</v>
+      </c>
+      <c r="B90" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>237</v>
+      </c>
+      <c r="B91" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>238</v>
+      </c>
+      <c r="B92" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>239</v>
+      </c>
+      <c r="B93" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>240</v>
+      </c>
+      <c r="B94" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>241</v>
+      </c>
+      <c r="B95" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>242</v>
+      </c>
+      <c r="B96" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>243</v>
+      </c>
+      <c r="B97" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>244</v>
+      </c>
+      <c r="B98" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>245</v>
+      </c>
+      <c r="B99" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>246</v>
+      </c>
+      <c r="B100" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15E01D2C-F4EB-0042-B649-9A2D35D8B08E}">
   <dimension ref="A1:A27"/>
   <sheetViews>
@@ -12556,4 +13980,1019 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C56C86FD-8286-414D-AD6F-6608D0E31C13}">
+  <dimension ref="A2:A201"/>
+  <sheetViews>
+    <sheetView topLeftCell="A177" workbookViewId="0">
+      <selection activeCell="A202" sqref="A202"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added cross validated testing
</commit_message>
<xml_diff>
--- a/analysis/naive/safe_write_predictions_naive.xlsx
+++ b/analysis/naive/safe_write_predictions_naive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fac_rubin/Documents/GeorgiaTech/CS_6727-Practicum/filesystem/analysis/naive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2C90BB-FD88-4E48-9A01-4DD802E7BD1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5590ABD-FD4F-544A-96E2-1A18D4162A08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9200" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{C6D897B8-16C8-7A4E-92A5-749E23A3A761}"/>
+    <workbookView xWindow="17680" yWindow="500" windowWidth="19560" windowHeight="19360" activeTab="1" xr2:uid="{C6D897B8-16C8-7A4E-92A5-749E23A3A761}"/>
   </bookViews>
   <sheets>
     <sheet name="runtime" sheetId="3" r:id="rId1"/>
@@ -1152,7 +1152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AD2641-593D-524F-A62F-7E528F7475AA}">
   <dimension ref="A1:F1459"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -12861,8 +12861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1302855-714D-1048-9062-B5A4A4F813DB}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>